<commit_message>
Added the computation of indices to find specific epochs to compute PSD, eg, touch_Go and preSC1
</commit_message>
<xml_diff>
--- a/docs/ephydataset_info_modified.xlsx
+++ b/docs/ephydataset_info_modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/work/comco/nandi.n/LFP_timescales/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB928ED-06BD-7249-B404-9EB9B117AFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0CFB4C-9755-EB41-B843-2A6ACBF2AD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="154">
   <si>
     <t>t150327002</t>
   </si>
@@ -348,9 +348,6 @@
     <t>L23:1-10, L5:11-15, L6:16-24</t>
   </si>
   <si>
-    <t>PMD</t>
-  </si>
-  <si>
     <t>t140924003</t>
   </si>
   <si>
@@ -484,13 +481,19 @@
   </si>
   <si>
     <t>L23:1-14, L5:15-23, L6:24-24</t>
+  </si>
+  <si>
+    <t>qualiity mentioned as 3 in new betaband lists by Bjorg</t>
+  </si>
+  <si>
+    <t>Cannot determine depth reliably in probe 1 - info in Laminar reconstruction Mourad .docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,6 +591,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -697,7 +708,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -767,6 +778,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
@@ -1090,9 +1115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S65" sqref="S65"/>
+      <selection pane="bottomLeft" activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1114,10 +1139,11 @@
     <col min="16" max="16" width="8.83203125" customWidth="1"/>
     <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="50.1640625" customWidth="1"/>
-    <col min="19" max="20" width="8.83203125" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" customWidth="1"/>
+    <col min="20" max="20" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" ht="26">
+    <row r="1" spans="1:20" s="6" customFormat="1" ht="26">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1176,7 +1202,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="7" customFormat="1" ht="22">
+    <row r="2" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A2" s="7" t="s">
         <v>89</v>
       </c>
@@ -1235,7 +1261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="7" customFormat="1" ht="22">
+    <row r="3" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A3" s="7" t="s">
         <v>92</v>
       </c>
@@ -1294,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="7" customFormat="1" ht="22">
+    <row r="4" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A4" s="7" t="s">
         <v>94</v>
       </c>
@@ -1353,7 +1379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="7" customFormat="1" ht="22">
+    <row r="5" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A5" s="7" t="s">
         <v>96</v>
       </c>
@@ -1412,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="6" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1471,7 +1497,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="7" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1530,7 +1556,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="8" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -1589,7 +1615,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="9" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -1648,7 +1674,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A10" s="7" t="s">
         <v>40</v>
       </c>
@@ -1707,66 +1733,69 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="12" customFormat="1" ht="22">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:20" s="31" customFormat="1" ht="22">
+      <c r="A11" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="8" t="s">
+      <c r="B11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="20">
         <v>32</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N11" s="8">
+      <c r="M11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="20">
         <v>-3.5</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="20">
         <v>-0.5</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q11" s="8">
+      <c r="P11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="20">
         <v>0.15</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="S11" s="11" t="s">
+      <c r="R11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="29" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" s="7" customFormat="1" ht="22">
+      <c r="T11" s="32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -1821,7 +1850,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="13" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -1880,7 +1909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="7" customFormat="1" ht="22">
+    <row r="14" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A14" s="7" t="s">
         <v>99</v>
       </c>
@@ -1939,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="7" customFormat="1" ht="22">
+    <row r="15" spans="1:20" s="7" customFormat="1" ht="22">
       <c r="A15" s="7" t="s">
         <v>101</v>
       </c>
@@ -1998,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="12" customFormat="1" ht="22">
+    <row r="16" spans="1:20" s="12" customFormat="1" ht="22">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
@@ -2414,7 +2443,7 @@
         <v>0.15</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>104</v>
@@ -2473,7 +2502,7 @@
         <v>0.15</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>18</v>
@@ -2530,7 +2559,7 @@
         <v>0.15</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>30</v>
@@ -2589,7 +2618,7 @@
         <v>0.15</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>18</v>
@@ -2648,7 +2677,7 @@
         <v>0.15</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>20</v>
@@ -2705,7 +2734,7 @@
         <v>0.15</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>20</v>
@@ -2762,7 +2791,7 @@
         <v>0.2</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>5</v>
@@ -2821,7 +2850,7 @@
         <v>0.15</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>20</v>
@@ -2880,7 +2909,7 @@
         <v>0.15</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>18</v>
@@ -2937,7 +2966,7 @@
         <v>0.15</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K32" s="8" t="s">
         <v>30</v>
@@ -2994,7 +3023,7 @@
         <v>0.15</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>30</v>
@@ -3053,7 +3082,7 @@
         <v>0.15</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>30</v>
@@ -3112,7 +3141,7 @@
         <v>0.15</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>20</v>
@@ -3165,13 +3194,13 @@
     </row>
     <row r="37" spans="1:20" ht="22">
       <c r="A37" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D37" s="8">
         <v>24</v>
@@ -3224,13 +3253,13 @@
     </row>
     <row r="38" spans="1:20" ht="22">
       <c r="A38" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D38" s="8">
         <v>24</v>
@@ -3283,13 +3312,13 @@
     </row>
     <row r="39" spans="1:20" ht="22">
       <c r="A39" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="8">
         <v>24</v>
@@ -3340,13 +3369,13 @@
     </row>
     <row r="40" spans="1:20" ht="22">
       <c r="A40" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D40" s="8">
         <v>24</v>
@@ -3399,13 +3428,13 @@
     </row>
     <row r="41" spans="1:20" ht="22">
       <c r="A41" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D41" s="8">
         <v>24</v>
@@ -3458,13 +3487,13 @@
     </row>
     <row r="42" spans="1:20" ht="22">
       <c r="A42" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D42" s="8">
         <v>24</v>
@@ -3517,13 +3546,13 @@
     </row>
     <row r="43" spans="1:20" ht="22">
       <c r="A43" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D43" s="8">
         <v>24</v>
@@ -3576,13 +3605,13 @@
     </row>
     <row r="44" spans="1:20" ht="22">
       <c r="A44" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D44" s="8">
         <v>24</v>
@@ -3635,13 +3664,13 @@
     </row>
     <row r="45" spans="1:20" s="26" customFormat="1" ht="22">
       <c r="A45" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D45" s="22">
         <v>24</v>
@@ -3692,18 +3721,18 @@
         <v>78</v>
       </c>
       <c r="T45" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="22">
       <c r="A46" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" s="8">
         <v>24</v>
@@ -3756,13 +3785,13 @@
     </row>
     <row r="47" spans="1:20" ht="22">
       <c r="A47" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D47" s="8">
         <v>24</v>
@@ -3815,13 +3844,13 @@
     </row>
     <row r="48" spans="1:20" ht="22">
       <c r="A48" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" s="8">
         <v>24</v>
@@ -3845,7 +3874,7 @@
         <v>2</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L48" s="8">
         <v>24</v>
@@ -3874,13 +3903,13 @@
     </row>
     <row r="49" spans="1:26" ht="22">
       <c r="A49" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" s="8">
         <v>24</v>
@@ -3904,7 +3933,7 @@
         <v>2</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L49" s="8">
         <v>24</v>
@@ -3933,13 +3962,13 @@
     </row>
     <row r="50" spans="1:26" ht="22">
       <c r="A50" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D50" s="8">
         <v>24</v>
@@ -3963,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L50" s="8">
         <v>24</v>
@@ -3992,13 +4021,13 @@
     </row>
     <row r="51" spans="1:26" ht="22">
       <c r="A51" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" s="22">
         <v>24</v>
@@ -4022,7 +4051,7 @@
         <v>2</v>
       </c>
       <c r="K51" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L51" s="22">
         <v>24</v>
@@ -4049,7 +4078,7 @@
         <v>78</v>
       </c>
       <c r="T51" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U51" s="26"/>
       <c r="V51" s="26"/>
@@ -4060,13 +4089,13 @@
     </row>
     <row r="52" spans="1:26" ht="22">
       <c r="A52" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D52" s="8">
         <v>24</v>
@@ -4090,7 +4119,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L52" s="8">
         <v>24</v>
@@ -4119,7 +4148,7 @@
     </row>
     <row r="53" spans="1:26" ht="22">
       <c r="A53" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>5</v>
@@ -4149,7 +4178,7 @@
         <v>2</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L53" s="8">
         <v>24</v>
@@ -4173,18 +4202,21 @@
         <v>5</v>
       </c>
       <c r="S53" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="T53" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="22">
       <c r="A54" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D54" s="22">
         <v>24</v>
@@ -4205,10 +4237,10 @@
         <v>0.2</v>
       </c>
       <c r="J54" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K54" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L54" s="22">
         <v>24</v>
@@ -4307,7 +4339,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D56" s="8">
         <v>24</v>
@@ -4331,7 +4363,7 @@
         <v>2</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L56" s="8">
         <v>24</v>
@@ -4366,7 +4398,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D57" s="8">
         <v>24</v>
@@ -4390,7 +4422,7 @@
         <v>2</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L57" s="8">
         <v>24</v>
@@ -4419,13 +4451,13 @@
     </row>
     <row r="58" spans="1:26" ht="22">
       <c r="A58" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D58" s="8">
         <v>24</v>
@@ -4449,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L58" s="8">
         <v>24</v>
@@ -4484,7 +4516,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D59" s="8">
         <v>24</v>
@@ -4505,10 +4537,10 @@
         <v>0.2</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L59" s="8">
         <v>24</v>
@@ -4543,7 +4575,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D60" s="8">
         <v>24</v>
@@ -4567,7 +4599,7 @@
         <v>2</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L60" s="8">
         <v>24</v>
@@ -4602,7 +4634,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D61" s="8">
         <v>24</v>
@@ -4623,10 +4655,10 @@
         <v>0.2</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L61" s="8">
         <v>24</v>
@@ -4661,7 +4693,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D62" s="8">
         <v>24</v>
@@ -4685,7 +4717,7 @@
         <v>2</v>
       </c>
       <c r="K62" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L62" s="8">
         <v>24</v>
@@ -4714,13 +4746,13 @@
     </row>
     <row r="63" spans="1:26" ht="22">
       <c r="A63" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D63" s="8">
         <v>24</v>
@@ -4741,10 +4773,10 @@
         <v>0.2</v>
       </c>
       <c r="J63" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L63" s="8">
         <v>24</v>
@@ -4773,13 +4805,13 @@
     </row>
     <row r="64" spans="1:26" ht="22">
       <c r="A64" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D64" s="8">
         <v>24</v>

</xml_diff>